<commit_message>
adding all in src
</commit_message>
<xml_diff>
--- a/data/Gule selskaber.xlsx
+++ b/data/Gule selskaber.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viggo\Desktop\Kaare\Samlet regneark\Gule selskaber\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gravercentret-my.sharepoint.com/personal/anja_gravercentret_dk/Documents/Dokumenter/Python_projekter/kommune_investering/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78CDEB59-D4B6-4FF1-9CF4-0C04C246C63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{78CDEB59-D4B6-4FF1-9CF4-0C04C246C63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B429F84-BCFD-4FAB-A051-1DA735DC7A77}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C4B3DE3D-2785-4267-A8BD-146C6FB57554}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C4B3DE3D-2785-4267-A8BD-146C6FB57554}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -1496,18 +1496,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D62E292E-E00C-4D8C-8A57-D34A07D2670D}">
   <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" customWidth="1"/>
-    <col min="3" max="3" width="31.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>30</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>44</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>46</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>48</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>53</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>56</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>59</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>62</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>65</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>68</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>71</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>76</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>79</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>82</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>85</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>87</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>90</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>93</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>96</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>99</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>101</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>103</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>107</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>110</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>113</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>115</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>118</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>121</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>124</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>126</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>128</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>131</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>134</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>136</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>138</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>140</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>142</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>145</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>148</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>150</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>153</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>156</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
         <v>158</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>161</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>163</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>166</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>169</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>172</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>177</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
         <v>178</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>181</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>183</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>185</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>187</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
         <v>189</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
         <v>192</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
         <v>195</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>198</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
         <v>200</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
         <v>203</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>206</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>208</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
         <v>210</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>212</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>214</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>217</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>219</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>222</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>224</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>226</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>228</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>231</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
         <v>233</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>236</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
         <v>238</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>241</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>243</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>246</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>248</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>251</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="s">
         <v>254</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>257</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>259</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>261</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>263</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>266</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
         <v>268</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>271</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>273</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>275</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>278</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="s">
         <v>281</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="20" t="s">
         <v>284</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>287</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>289</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>291</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>293</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>295</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>297</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>300</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>302</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>305</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>308</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>310</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>312</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>314</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>318</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>319</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>321</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>324</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>326</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>328</v>
       </c>

</xml_diff>